<commit_message>
Update Stakeholderanalyse - v2.xlsx
</commit_message>
<xml_diff>
--- a/Stakeholderanalyse - v2.xlsx
+++ b/Stakeholderanalyse - v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\EPWS2223HausenKochZimmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B347A9F-6205-4CAA-819C-F630D0627A70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D655E0-E552-41A3-8E13-E6E1E2D1B0EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1EC1A410-8258-43E6-AE3C-02DE8233B07A}"/>
   </bookViews>
@@ -590,49 +590,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -644,36 +614,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +690,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -995,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0898466-D973-4392-B5CB-258D34DDA08A}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1010,364 +1006,364 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="9" t="s">
+      <c r="A4" s="31"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9" t="s">
+      <c r="A5" s="31"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="9" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="9" t="s">
+      <c r="A7" s="31"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="29" t="s">
+      <c r="A8" s="31"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="29" t="s">
+      <c r="A9" s="31"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="29"/>
+      <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="26" t="s">
+      <c r="A10" s="31"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="10"/>
+      <c r="A11" s="31"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="30"/>
       <c r="D11" s="30"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="9" t="s">
+      <c r="B14" s="39"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="28" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10"/>
-      <c r="C16" s="33" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="30"/>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="35" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="36"/>
+      <c r="F18" s="23"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="35" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="36"/>
+      <c r="F19" s="23"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="29" t="s">
+      <c r="B20" s="34"/>
+      <c r="C20" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="35" t="s">
+      <c r="D20" s="29"/>
+      <c r="E20" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="36"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="17"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="28" t="s">
+      <c r="B23" s="34"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="17"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="9" t="s">
+      <c r="B24" s="34"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="17"/>
-      <c r="C25" s="29" t="s">
+      <c r="B25" s="34"/>
+      <c r="C25" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="9" t="s">
+      <c r="D25" s="29"/>
+      <c r="E25" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="17"/>
+      <c r="B26" s="34"/>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="9" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="5" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="9" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="40"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="27" t="s">
+      <c r="E31" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="31" t="s">
+      <c r="C32" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="38" t="s">
+      <c r="E32" s="24" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="37"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="17"/>
-      <c r="C34" s="34" t="s">
+      <c r="B34" s="34"/>
+      <c r="C34" s="21" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="30"/>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1375,42 +1371,53 @@
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="21" t="s">
+      <c r="B35" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="22"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C36" s="32"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="22"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="22"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="21" t="s">
+      <c r="B38" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="22"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="5"/>
+      <c r="B39" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="C32:C33"/>
     <mergeCell ref="D32:D34"/>
     <mergeCell ref="A27:A30"/>
@@ -1422,19 +1429,8 @@
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="B32:B34"/>
-    <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D16"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>